<commit_message>
feat: updated attribute sheet
</commit_message>
<xml_diff>
--- a/IGM_attribute_2.0.0.xlsx
+++ b/IGM_attribute_2.0.0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="187">
   <si>
     <t>Path</t>
   </si>
@@ -514,13 +514,13 @@
     <t>I1</t>
   </si>
   <si>
-    <t>Describes the item details for resolution details</t>
+    <t>Refers to the item for which the resolution has been provided</t>
   </si>
   <si>
     <t>message.issue.resolutions.tags.RESOLUTION_DETAILS.list.REFUND_AMOUNT</t>
   </si>
   <si>
-    <t>Describes the refund amount for resolution details</t>
+    <t>Refers to the amount being provided as refund. Applicable in case refund amount is to be provided resolutions such as REFUND or CANCEL</t>
   </si>
   <si>
     <t>message.issue.refs.tags.message.order.items</t>
@@ -532,7 +532,7 @@
     <t>message.issue.refs.tags.message.order.items.list.quantity.selected.count</t>
   </si>
   <si>
-    <t>Describes the selected quantity</t>
+    <t xml:space="preserve">Used to specify the quantity of the item selected for the complaint. Example 2 out of 3 quantity shirts have defect. </t>
   </si>
   <si>
     <t>message.issue.actions.tags.CLOSURE_DETAILS</t>
@@ -544,7 +544,10 @@
     <t>message.issue.actions.tags.CLOSURE_DETAILS.RATING</t>
   </si>
   <si>
-    <t>Describes the tag as Rating</t>
+    <t>THUMBS-UP</t>
+  </si>
+  <si>
+    <t>Refers to the rating provided by the buyer at the complaint closure</t>
   </si>
   <si>
     <t>on_issue</t>
@@ -633,12 +636,12 @@
       <name val="Arial"/>
     </font>
     <font>
-      <color rgb="FF212529"/>
+      <u/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF212529"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -717,17 +720,17 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2490,10 +2493,10 @@
         <v>9</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2909,7 +2912,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>35</v>
@@ -3277,7 +3280,7 @@
         <v>73</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24">
@@ -3482,7 +3485,7 @@
     </row>
     <row r="34">
       <c r="A34" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>7</v>
@@ -3494,7 +3497,7 @@
         <v>9</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>106</v>
@@ -3654,7 +3657,7 @@
         <v>9</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>129</v>
@@ -3921,23 +3924,23 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="B58" s="2" t="s">
+      <c r="A58" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="2" t="s">
+      <c r="C58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="F58" s="2" t="s">
-        <v>170</v>
+      <c r="F58" s="5" t="s">
+        <v>163</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -3962,23 +3965,23 @@
       <c r="AA58" s="2"/>
     </row>
     <row r="59">
-      <c r="A59" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="B59" s="2" t="s">
+      <c r="A59" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="19">
-        <v>2.0</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>172</v>
+      <c r="C59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>166</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -4004,7 +4007,7 @@
     </row>
     <row r="60">
       <c r="A60" s="7" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>111</v>
@@ -4015,16 +4018,16 @@
       <c r="D60" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E60" s="5" t="s">
-        <v>162</v>
+      <c r="E60" s="5">
+        <v>200.0</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="7" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>111</v>
@@ -4036,15 +4039,15 @@
         <v>9</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="7" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>111</v>
@@ -4056,11 +4059,27 @@
         <v>9</v>
       </c>
       <c r="E62" s="5">
-        <v>200.0</v>
+        <v>2.0</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>168</v>
-      </c>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="7"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="7"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4138,7 +4157,7 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -4179,7 +4198,7 @@
       <c r="AA2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -4232,7 +4251,7 @@
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="18" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -4314,7 +4333,7 @@
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="19" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -4358,7 +4377,7 @@
       <c r="E7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="18" t="s">
         <v>26</v>
       </c>
       <c r="G7" s="2"/>
@@ -4425,22 +4444,22 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="18" t="s">
         <v>32</v>
       </c>
       <c r="G9" s="2"/>
@@ -4478,10 +4497,10 @@
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="F10" s="20" t="s">
+      <c r="E10" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>35</v>
       </c>
       <c r="G10" s="2"/>
@@ -4519,7 +4538,7 @@
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="19" t="s">
         <v>37</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -4601,7 +4620,7 @@
       <c r="D13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="19" t="s">
         <v>44</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -4642,7 +4661,7 @@
       <c r="D14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="19" t="s">
         <v>47</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -4672,7 +4691,7 @@
     </row>
     <row r="15">
       <c r="A15" s="14" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>7</v>
@@ -4687,7 +4706,7 @@
         <v>165</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -5099,7 +5118,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>35</v>
@@ -5427,7 +5446,7 @@
         <v>73</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22">
@@ -5632,7 +5651,7 @@
     </row>
     <row r="32">
       <c r="A32" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>7</v>
@@ -5644,7 +5663,7 @@
         <v>9</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>106</v>
@@ -5804,7 +5823,7 @@
         <v>9</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>129</v>
@@ -6071,24 +6090,12 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>170</v>
-      </c>
+      <c r="A54" s="20"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -6112,24 +6119,12 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55">
-      <c r="A55" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="19">
-        <v>2.0</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>172</v>
-      </c>
+      <c r="A55" s="20"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -6152,6 +6147,146 @@
       <c r="Z55" s="2"/>
       <c r="AA55" s="2"/>
     </row>
+    <row r="57">
+      <c r="A57" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="5">
+        <v>200.0</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="E6"/>

</xml_diff>